<commit_message>
Cleaning code up. Added excel results parsing file
</commit_message>
<xml_diff>
--- a/results-summary.xlsx
+++ b/results-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codebase\ml-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA12819A-D85B-48F1-9011-FD94FA9054E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851BA2A-3823-4C9A-A69F-36A62D2C303D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040" activeTab="2" xr2:uid="{8CDA145B-ED62-43F3-8180-ADC43FD7B724}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040" activeTab="2" xr2:uid="{8CDA145B-ED62-43F3-8180-ADC43FD7B724}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -244,7 +244,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,14 +1153,14 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E25"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43.5703125" bestFit="1" customWidth="1"/>

</xml_diff>